<commit_message>
Update Stanleys Abenteuer Aufgaben 20.01.2023.xlsx
</commit_message>
<xml_diff>
--- a/Assets/Documents/Stanleys Abenteuer Aufgaben 20.01.2023.xlsx
+++ b/Assets/Documents/Stanleys Abenteuer Aufgaben 20.01.2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\GitHub\HangedLarryStan\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D45249E-F8CE-4055-858A-BB9C6242CE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736D34FE-066C-4527-AF44-36408A511CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>Stanleys Abenteuer Präsentation</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Fertig</t>
+  </si>
+  <si>
+    <t>In Arbeit</t>
+  </si>
+  <si>
+    <t>Wartet</t>
   </si>
 </sst>
 </file>
@@ -537,6 +543,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -567,12 +594,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -581,21 +602,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,7 +886,7 @@
   <dimension ref="A2:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,14 +905,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -945,13 +951,13 @@
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:10" s="8" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
     </row>
     <row r="13" spans="1:10" s="5" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
@@ -975,96 +981,102 @@
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="20" t="s">
         <v>14</v>
       </c>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="23" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="28" t="s">
+      <c r="E15" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="33" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="27" t="s">
+      <c r="A16" s="24"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="29"/>
+      <c r="E16" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="35" t="s">
+      <c r="A17" s="24"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="29"/>
+      <c r="F17" s="34"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="27" t="s">
+      <c r="A18" s="24"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="29"/>
+      <c r="E18" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="34"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="34" t="s">
+      <c r="A19" s="24"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="30"/>
+      <c r="F19" s="35"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="9" t="s">
         <v>40</v>
       </c>
@@ -1075,14 +1087,14 @@
         <v>35</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="9" t="s">
@@ -1095,14 +1107,14 @@
         <v>36</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="9" t="s">
         <v>19</v>
       </c>
@@ -1113,14 +1125,14 @@
         <v>37</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="13" t="s">
         <v>21</v>
       </c>
@@ -1131,7 +1143,7 @@
         <v>36</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>22</v>

</xml_diff>